<commit_message>
updated job_data 31 pages
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CE2147E-33A6-49AA-8D4E-59BAAFEC3691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E872559-528B-470B-9FA5-3693BC56E86C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5595" yWindow="1755" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing Plan Data" sheetId="1" r:id="rId1"/>
@@ -584,6 +584,57 @@
       <font>
         <b val="0"/>
         <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Euphemia"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Euphemia"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Euphemia"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <color theme="4" tint="-0.499984740745262"/>
       </font>
       <fill>
@@ -675,57 +726,6 @@
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Euphemia"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Euphemia"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Euphemia"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -830,7 +830,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="285751" y="695321"/>
+          <a:off x="314326" y="695321"/>
           <a:ext cx="2286000" cy="274320"/>
           <a:chOff x="200026" y="847725"/>
           <a:chExt cx="2009774" cy="274320"/>
@@ -1035,8 +1035,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="285749" y="695325"/>
-          <a:ext cx="2105025" cy="274320"/>
+          <a:off x="314324" y="695325"/>
+          <a:ext cx="2286000" cy="274320"/>
           <a:chOff x="200024" y="981075"/>
           <a:chExt cx="2097896" cy="274320"/>
         </a:xfrm>
@@ -1219,10 +1219,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Data" displayName="Data" ref="B5:I15">
   <autoFilter ref="B5:I15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TASK" totalsRowLabel="Total" totalsRowDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TASK" totalsRowLabel="Total" totalsRowDxfId="2"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="STATUS" totalsRowFunction="count"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="OWNER" totalsRowDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="ASSIGNED TO" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="OWNER" totalsRowDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="ASSIGNED TO" totalsRowDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ANTICIPATED_x000a_START DATE" dataCellStyle="Date"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ANTICIPATED_x000a_END DATE" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ACTUAL _x000a_START DATE " dataCellStyle="Date"/>
@@ -1525,18 +1525,18 @@
   </sheetPr>
   <dimension ref="B1:I15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="39.5" style="3" customWidth="1"/>
-    <col min="3" max="4" width="14.375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.875" style="3" customWidth="1"/>
-    <col min="6" max="9" width="15.375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="2.625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.44140625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="14.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="3" customWidth="1"/>
+    <col min="6" max="9" width="15.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1552,7 +1552,7 @@
       <c r="H1" s="25"/>
       <c r="I1" s="25"/>
     </row>
-    <row r="2" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="26" t="s">
         <v>14</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="24"/>
       <c r="D4" s="7" t="s">
         <v>5</v>
@@ -1606,7 +1606,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="21" t="s">
         <v>7</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="18" t="s">
         <v>21</v>
       </c>
@@ -1656,12 +1656,12 @@
       </c>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>24</v>
@@ -1675,10 +1675,14 @@
       <c r="G7" s="20">
         <v>43998</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-    </row>
-    <row r="8" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="20">
+        <v>43997</v>
+      </c>
+      <c r="I7" s="20">
+        <v>43998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="18" t="s">
         <v>30</v>
       </c>
@@ -1700,7 +1704,7 @@
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="18" t="s">
         <v>31</v>
       </c>
@@ -1722,7 +1726,7 @@
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="18" t="s">
         <v>28</v>
       </c>
@@ -1744,7 +1748,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="18" t="s">
         <v>29</v>
       </c>
@@ -1766,7 +1770,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="18" t="s">
         <v>32</v>
       </c>
@@ -1788,7 +1792,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="18" t="s">
         <v>33</v>
       </c>
@@ -1810,7 +1814,7 @@
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="18" t="s">
         <v>34</v>
       </c>
@@ -1832,7 +1836,7 @@
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="18" t="s">
         <v>35</v>
       </c>
@@ -1856,30 +1860,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:I15">
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="10" priority="15">
       <formula>(clCustom2="ON")*($C6=txtCustom2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="16">
+    <cfRule type="expression" dxfId="9" priority="16">
       <formula>(clCustom3="ON")*($C6=txtCustom3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="17">
+    <cfRule type="expression" dxfId="8" priority="17">
       <formula>(clCustom4="ON")*($C6=txtCustom4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:I15">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>($C6="Not Started")*(clNotStarted="ON")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>($C6="In Progress")*(clInProgress="ON")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>($C6="Delayed")*(clDelayed="ON")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="12">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>($C6="Complete")*(clComplete="ON")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="14">
+    <cfRule type="expression" dxfId="3" priority="14">
       <formula>(clCustom1="ON")*($C6=txtCustom1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1943,20 +1947,20 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="18.875" customWidth="1"/>
-    <col min="3" max="3" width="25.375" customWidth="1"/>
-    <col min="4" max="4" width="2.625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
@@ -1970,43 +1974,43 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
@@ -2246,20 +2250,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2282,6 +2286,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF76A04A-2A1F-4BD3-A173-1A19CE9CC2C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D29A437-0917-4D06-BCBA-61F405397D21}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2289,12 +2301,4 @@
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF76A04A-2A1F-4BD3-A173-1A19CE9CC2C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update project plan including Presentation outline
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E872559-528B-470B-9FA5-3693BC56E86C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874E76A6-DD45-4CB1-81FB-04C6484B43D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="1755" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing Plan Data" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t>Marketing Plan Data</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Question(skills) - optional</t>
+  </si>
+  <si>
+    <t>Presentation outline</t>
   </si>
 </sst>
 </file>
@@ -1216,8 +1219,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Data" displayName="Data" ref="B5:I15">
-  <autoFilter ref="B5:I15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Data" displayName="Data" ref="B5:I16">
+  <autoFilter ref="B5:I16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TASK" totalsRowLabel="Total" totalsRowDxfId="2"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="STATUS" totalsRowFunction="count"/>
@@ -1523,10 +1526,10 @@
     <tabColor theme="4" tint="0.39997558519241921"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I15"/>
+  <dimension ref="B1:I16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1637,7 +1640,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>22</v>
@@ -1654,7 +1657,9 @@
       <c r="H6" s="20">
         <v>43995</v>
       </c>
-      <c r="I6" s="20"/>
+      <c r="I6" s="20">
+        <v>43998</v>
+      </c>
     </row>
     <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="18" t="s">
@@ -1696,10 +1701,10 @@
         <v>25</v>
       </c>
       <c r="F8" s="20">
-        <v>43998</v>
+        <v>43999</v>
       </c>
       <c r="G8" s="20">
-        <v>43999</v>
+        <v>44000</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
@@ -1718,10 +1723,10 @@
         <v>26</v>
       </c>
       <c r="F9" s="20">
-        <v>43998</v>
+        <v>43999</v>
       </c>
       <c r="G9" s="20">
-        <v>43999</v>
+        <v>44000</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
@@ -1772,60 +1777,60 @@
     </row>
     <row r="12" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="18" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="20">
         <v>44000</v>
       </c>
       <c r="G12" s="20">
-        <v>44001</v>
+        <v>44002</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="20">
+        <v>44000</v>
+      </c>
+      <c r="G13" s="20">
         <v>44001</v>
-      </c>
-      <c r="G13" s="20">
-        <v>44002</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
     </row>
     <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F14" s="20">
         <v>44001</v>
@@ -1838,28 +1843,50 @@
     </row>
     <row r="15" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="20">
+        <v>44001</v>
+      </c>
+      <c r="G15" s="20">
         <v>44002</v>
-      </c>
-      <c r="G15" s="20">
-        <v>44003</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
     </row>
+    <row r="16" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="20">
+        <v>44002</v>
+      </c>
+      <c r="G16" s="20">
+        <v>44003</v>
+      </c>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B6:I15">
+  <conditionalFormatting sqref="B6:I16">
     <cfRule type="expression" dxfId="10" priority="15">
       <formula>(clCustom2="ON")*($C6=txtCustom2)</formula>
     </cfRule>
@@ -1870,7 +1897,7 @@
       <formula>(clCustom4="ON")*($C6=txtCustom4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:I15">
+  <conditionalFormatting sqref="B6:I16">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>($C6="Not Started")*(clNotStarted="ON")</formula>
     </cfRule>
@@ -1908,13 +1935,13 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Customize a new status category in this cell. Select On or Off in cell below to toggle row highlight for this status" sqref="H3:I3" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Select cell below to navigate to List Data worksheet. Status categories are in cells D3 through K4" sqref="B1:C1" xr:uid="{00000000-0002-0000-0000-000015000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Status categories are defined in cells D3 to K4. Customize Status categories to match the marketing plan data. Select On or Off in cell below to toggle row highlight" sqref="H1:I1 D1:F1" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Assigned to name from the list. Select CANCEL, then press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="E6:E15" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Assigned to name from the list. Select CANCEL, then press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="E6:E16" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Names</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Owner name from the list. Select CANCEL, then press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="D6:D15" xr:uid="{00000000-0002-0000-0000-000016000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Owner name from the list. Select CANCEL, then press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="D6:D16" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>Names</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Status from the list. Select CANCEL, then press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="C6:C15" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Status from the list. Select CANCEL, then press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="C6:C16" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$D$3:$I$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -2039,6 +2066,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9677210f24a1be23c92c90fd886aa0aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e05723c5c1908df1a1a4ebf11d344e" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -2249,24 +2293,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF76A04A-2A1F-4BD3-A173-1A19CE9CC2C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D29A437-0917-4D06-BCBA-61F405397D21}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ECA9EA0-A96C-480C-BDE5-8B712DE09016}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2283,22 +2328,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF76A04A-2A1F-4BD3-A173-1A19CE9CC2C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D29A437-0917-4D06-BCBA-61F405397D21}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>